<commit_message>
Criado arquivo operação com uma forma mais completa de desenhar
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D5B060D-123B-466C-B60E-0860735D3272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176A73E4-85E8-4077-8AC8-F971B92836B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="17295" windowHeight="8685" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>notas</t>
+  </si>
+  <si>
+    <t>MODELO</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -413,8 +416,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1172009309</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Atualização de parametros de desenho
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{176A73E4-85E8-4077-8AC8-F971B92836B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6808FC-4979-4363-9E17-F38B6EACCE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="17295" windowHeight="8685" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>notas</t>
-  </si>
-  <si>
-    <t>MODELO</t>
   </si>
 </sst>
 </file>
@@ -402,7 +399,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,8 +413,8 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>2000049503</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
iniciação do modulo recondutoramento
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6808FC-4979-4363-9E17-F38B6EACCE4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B3484A-C7CA-4770-8FD5-E90154E76148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15840" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -18,18 +18,10 @@
     <sheet name="Planilha3" sheetId="3" r:id="rId3"/>
     <sheet name="Planilha4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -396,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D683FFD3-73CE-42DD-AF4E-11C18A4FE4C7}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,11 +406,18 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2000049503</v>
+        <v>2000033005</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2">
+        <v>2000033006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>2000062283</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
atualização do modulo recondutoramento
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B3484A-C7CA-4770-8FD5-E90154E76148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFB8247-989F-453C-B3CD-818437BD78FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="18300" windowHeight="11040" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D683FFD3-73CE-42DD-AF4E-11C18A4FE4C7}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,17 +406,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2000033005</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2000033006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>2000062283</v>
+        <v>2000056127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
insrecao do resultado do esforco
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFFB8247-989F-453C-B3CD-818437BD78FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015398F8-9261-43DE-B5EB-F459D6A49E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="18300" windowHeight="11040" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -388,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D683FFD3-73CE-42DD-AF4E-11C18A4FE4C7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,15 +399,27 @@
     <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>2000056127</v>
+        <v>2000056514</v>
       </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J3" s="2"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J6" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
ADICIONADO INSERÇÃO DE CHV FACA
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{015398F8-9261-43DE-B5EB-F459D6A49E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7883F-ADF8-4B38-9DF0-5EFBBCC45AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,9 +28,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>notas</t>
+  </si>
+  <si>
+    <t>1145623903 A</t>
+  </si>
+  <si>
+    <t>1145623903 B</t>
   </si>
 </sst>
 </file>
@@ -391,7 +397,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,11 +411,14 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>2000056514</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
INSERCAO DO CIRCULO, ANCO
</commit_message>
<xml_diff>
--- a/notas.xlsx
+++ b/notas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeuge\PycharmProjects\autopro\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F7883F-ADF8-4B38-9DF0-5EFBBCC45AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC96C121-472E-4509-822E-1B7618B75CF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
+    <workbookView xWindow="20370" yWindow="-4665" windowWidth="29040" windowHeight="15720" xr2:uid="{7DA2C87B-BA47-41B8-8124-F6BB0B7E3EF3}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -28,15 +28,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>notas</t>
-  </si>
-  <si>
-    <t>1145623903 A</t>
-  </si>
-  <si>
-    <t>1145623903 B</t>
   </si>
 </sst>
 </file>
@@ -72,11 +66,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -397,38 +388,38 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>2000049052</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
+      <c r="A3" s="1">
+        <v>2000049053</v>
       </c>
-      <c r="J3" s="2"/>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J4" s="2"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J5" s="2"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J6" s="2"/>
+      <c r="J6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>